<commit_message>
xong phần truyền tính hiệu...còn phần tạo pan
</commit_message>
<xml_diff>
--- a/Đo_An/HoanThanhDangNhap/bin/Debug/Resources3/Du lieu cau hoi/thu vien bai hoc.xlsx
+++ b/Đo_An/HoanThanhDangNhap/bin/Debug/Resources3/Du lieu cau hoi/thu vien bai hoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đăng_Quý_UTE_K19\Dang_Quy_UTE_k19\Đo_An\HoanThanhDangNhap\bin\Debug\Resources3\Du lieu cau hoi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF0E32C-B192-497E-A636-16A4BDB55518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61ABD55-FD5D-413A-950A-7D7B45CCF3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2400" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2445" uniqueCount="579">
   <si>
     <t>nActi</t>
   </si>
@@ -1795,12 +1795,42 @@
   <si>
     <t>Bài 13: Cảm biến bàn đạp ga kiểu phần tử hall</t>
   </si>
+  <si>
+    <t>Tên Đồ Thị</t>
+  </si>
+  <si>
+    <t>Mã Đồ Thị</t>
+  </si>
+  <si>
+    <t>@01D1#</t>
+  </si>
+  <si>
+    <t>ngu nhu con bòa</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>sdfsd</t>
+  </si>
+  <si>
+    <t>sfsdf</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>Mã chân cb</t>
+  </si>
+  <si>
+    <t>@01D2#</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1893,6 +1923,18 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1962,7 +2004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2027,9 +2069,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2042,6 +2081,13 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2360,10 +2406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2382,7 +2428,7 @@
     <col min="14" max="16384" width="12.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2422,11 +2468,23 @@
       <c r="M1" s="5" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="40" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="O1" s="40" t="s">
+        <v>569</v>
+      </c>
+      <c r="P1" s="40" t="s">
+        <v>570</v>
+      </c>
+      <c r="Q1" s="41" t="s">
+        <v>577</v>
+      </c>
+      <c r="R1" s="41" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
@@ -2436,7 +2494,7 @@
       <c r="C2" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>555</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -2469,8 +2527,20 @@
       <c r="N2" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>16</v>
       </c>
@@ -2480,7 +2550,7 @@
       <c r="C3" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>555</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -2496,7 +2566,7 @@
         <v>406</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>408</v>
+        <v>573</v>
       </c>
       <c r="J3" s="17" t="s">
         <v>12</v>
@@ -2513,8 +2583,20 @@
       <c r="N3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="O3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="42" t="s">
+        <v>571</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
@@ -2524,7 +2606,7 @@
       <c r="C4" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>555</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -2549,7 +2631,7 @@
         <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>408</v>
+        <v>14</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>14</v>
@@ -2557,8 +2639,20 @@
       <c r="N4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="O4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
@@ -2568,11 +2662,11 @@
       <c r="C5" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>555</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>404</v>
@@ -2581,19 +2675,19 @@
         <v>14</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>14</v>
+        <v>575</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>14</v>
+        <v>574</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K5" s="17" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>14</v>
+        <v>573</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>12</v>
@@ -2601,8 +2695,20 @@
       <c r="N5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="O5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>20</v>
       </c>
@@ -2612,7 +2718,7 @@
       <c r="C6" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="17" t="s">
@@ -2645,8 +2751,20 @@
       <c r="N6" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>28</v>
       </c>
@@ -2660,7 +2778,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="4"/>
@@ -2672,7 +2790,7 @@
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="4"/>
@@ -2684,7 +2802,7 @@
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="4"/>
@@ -2696,7 +2814,7 @@
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="4"/>
@@ -2708,7 +2826,7 @@
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="4"/>
@@ -2720,7 +2838,7 @@
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="4"/>
@@ -2732,7 +2850,7 @@
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="4"/>
@@ -2744,7 +2862,7 @@
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="4"/>
@@ -2756,7 +2874,7 @@
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="4"/>
@@ -2847,13 +2965,13 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="37" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2867,7 +2985,7 @@
       <c r="C2" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>565</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -2911,7 +3029,7 @@
       <c r="C3" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>565</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -2955,7 +3073,7 @@
       <c r="C4" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>565</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -2999,7 +3117,7 @@
       <c r="C5" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -3358,13 +3476,13 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="37" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3378,7 +3496,7 @@
       <c r="C2" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>566</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -3422,7 +3540,7 @@
       <c r="C3" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>566</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -3466,7 +3584,7 @@
       <c r="C4" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>566</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -3510,7 +3628,7 @@
       <c r="C5" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -3610,13 +3728,13 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="37" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3630,7 +3748,7 @@
       <c r="C2" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>567</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -3674,7 +3792,7 @@
       <c r="C3" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>567</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -3718,7 +3836,7 @@
       <c r="C4" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>567</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -3762,7 +3880,7 @@
       <c r="C5" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -3865,13 +3983,13 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="37" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3885,7 +4003,7 @@
       <c r="C2" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>568</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -3929,7 +4047,7 @@
       <c r="C3" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>568</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -3973,7 +4091,7 @@
       <c r="C4" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>568</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -4017,7 +4135,7 @@
       <c r="C5" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -4993,11 +5111,11 @@
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -5033,10 +5151,10 @@
       <c r="N2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="O2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="41"/>
+      <c r="P2" s="43"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -5072,10 +5190,10 @@
       <c r="N3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="41" t="s">
+      <c r="O3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="41"/>
+      <c r="P3" s="43"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -5111,10 +5229,10 @@
       <c r="N4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="41" t="s">
+      <c r="O4" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="41"/>
+      <c r="P4" s="43"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -8887,10 +9005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8909,7 +9027,7 @@
     <col min="14" max="16384" width="12.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -8952,9 +9070,17 @@
       <c r="N1" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="O1" s="36"/>
-    </row>
-    <row r="2" spans="1:15" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="O1" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
@@ -8964,7 +9090,7 @@
       <c r="C2" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>556</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -8997,8 +9123,17 @@
       <c r="N2" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>16</v>
       </c>
@@ -9008,7 +9143,7 @@
       <c r="C3" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>556</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -9041,8 +9176,17 @@
       <c r="N3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="O3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
@@ -9052,7 +9196,7 @@
       <c r="C4" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>556</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -9085,8 +9229,17 @@
       <c r="N4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="O4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
@@ -9096,7 +9249,7 @@
       <c r="C5" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>556</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -9129,8 +9282,17 @@
       <c r="N5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="O5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>20</v>
       </c>
@@ -9140,7 +9302,7 @@
       <c r="C6" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="39" t="s">
         <v>556</v>
       </c>
       <c r="E6" s="17" t="s">
@@ -9173,8 +9335,17 @@
       <c r="N6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="O6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>21</v>
       </c>
@@ -9184,7 +9355,7 @@
       <c r="C7" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="17" t="s">
@@ -9217,8 +9388,17 @@
       <c r="N7" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>28</v>
       </c>
@@ -9233,7 +9413,7 @@
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="4"/>
@@ -9246,7 +9426,7 @@
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="4"/>
@@ -9259,7 +9439,7 @@
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="4"/>
@@ -9272,7 +9452,7 @@
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="4"/>
@@ -9285,7 +9465,7 @@
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="4"/>
@@ -9298,7 +9478,7 @@
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="4"/>
@@ -9403,7 +9583,7 @@
       <c r="C2" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>557</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -9447,7 +9627,7 @@
       <c r="C3" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>557</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -9491,7 +9671,7 @@
       <c r="C4" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>557</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -9535,7 +9715,7 @@
       <c r="C5" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -9674,7 +9854,7 @@
       <c r="C2" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>558</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -9718,7 +9898,7 @@
       <c r="C3" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>558</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -9762,7 +9942,7 @@
       <c r="C4" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>558</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -9806,7 +9986,7 @@
       <c r="C5" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>558</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -9850,7 +10030,7 @@
       <c r="C6" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="17" t="s">
@@ -10002,13 +10182,13 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="L1" s="36" t="s">
         <v>396</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="M1" s="36" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="36" t="s">
         <v>397</v>
       </c>
     </row>
@@ -10022,7 +10202,7 @@
       <c r="C2" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>559</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -10066,7 +10246,7 @@
       <c r="C3" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>559</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -10110,7 +10290,7 @@
       <c r="C4" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -10217,13 +10397,13 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="37" t="s">
         <v>397</v>
       </c>
     </row>
@@ -10237,7 +10417,7 @@
       <c r="C2" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>560</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -10281,7 +10461,7 @@
       <c r="C3" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>560</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -10325,7 +10505,7 @@
       <c r="C4" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -10478,13 +10658,13 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="37" t="s">
         <v>397</v>
       </c>
     </row>
@@ -10498,7 +10678,7 @@
       <c r="C2" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>561</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -10542,7 +10722,7 @@
       <c r="C3" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>562</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -10586,7 +10766,7 @@
       <c r="C4" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>561</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -10630,7 +10810,7 @@
       <c r="C5" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -10920,13 +11100,13 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="37" t="s">
         <v>397</v>
       </c>
     </row>
@@ -10940,7 +11120,7 @@
       <c r="C2" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>563</v>
       </c>
       <c r="E2" s="18" t="s">
@@ -10985,7 +11165,7 @@
       <c r="C3" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>563</v>
       </c>
       <c r="E3" s="18" t="s">
@@ -11030,7 +11210,7 @@
       <c r="C4" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>563</v>
       </c>
       <c r="E4" s="18" t="s">
@@ -11075,7 +11255,7 @@
       <c r="C5" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>563</v>
       </c>
       <c r="E5" s="18" t="s">
@@ -11120,7 +11300,7 @@
       <c r="C6" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="18" t="s">
@@ -11445,13 +11625,13 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="38" t="s">
         <v>396</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="38" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="38" t="s">
         <v>397</v>
       </c>
     </row>
@@ -11465,7 +11645,7 @@
       <c r="C2" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>564</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -11509,7 +11689,7 @@
       <c r="C3" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>564</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -11553,7 +11733,7 @@
       <c r="C4" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>564</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -11597,7 +11777,7 @@
       <c r="C5" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="17" t="s">

</xml_diff>

<commit_message>
code mới fix lỗi câu 1 resources2 29.12.2023
</commit_message>
<xml_diff>
--- a/Đo_An/HoanThanhDangNhap/bin/Debug/Resources3/Du lieu cau hoi/thu vien bai hoc.xlsx
+++ b/Đo_An/HoanThanhDangNhap/bin/Debug/Resources3/Du lieu cau hoi/thu vien bai hoc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đồ án tốt nghiệp\doantn\27-12\Dang_Quy_UTE_k19\Đo_An\HoanThanhDangNhap\bin\Debug\Resources3\Du lieu cau hoi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đăng_Quý_UTE_K19\Đo_An\HoanThanhDangNhap\bin\Debug\Resources3\Du lieu cau hoi\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2B5DBE-CB16-466C-BC43-802EA44849B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="12"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="9" r:id="rId1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="624">
   <si>
     <t>nActi</t>
   </si>
@@ -1953,11 +1954,20 @@
   <si>
     <t>D. 1 là VCPA1, 2 là VCPA2, 3 là EPA1, 4 là EPA2, 5 là VPA1, 6 là VPA2</t>
   </si>
+  <si>
+    <t>@01D2#</t>
+  </si>
+  <si>
+    <t>@01D1#</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2514,11 +2524,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2676,7 +2686,7 @@
         <v>471</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>472</v>
+        <v>623</v>
       </c>
       <c r="J3" s="17" t="s">
         <v>12</v>
@@ -2700,10 +2710,10 @@
         <v>14</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>14</v>
+        <v>621</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -2812,10 +2822,10 @@
         <v>14</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>584</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2865,7 +2875,7 @@
         <v>581</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>582</v>
+        <v>622</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>14</v>
@@ -3011,11 +3021,11 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c1\\1.PNG"/>
-    <hyperlink ref="C3" r:id="rId2" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c1\\2.PNG"/>
-    <hyperlink ref="C4" r:id="rId3" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c1\\3.PNG"/>
-    <hyperlink ref="C5" r:id="rId4" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c1\\4.PNG"/>
-    <hyperlink ref="C6" r:id="rId5" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c1\\4.PNG"/>
+    <hyperlink ref="C2" r:id="rId1" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c1\\1.PNG" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c1\\2.PNG" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c1\\3.PNG" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c1\\4.PNG" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c1\\4.PNG" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -3023,7 +3033,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -3455,17 +3465,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4028,10 +4038,10 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -4039,7 +4049,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -4341,21 +4351,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4584,10 +4594,10 @@
         <v>14</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>91</v>
+        <v>621</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>584</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4637,7 +4647,7 @@
         <v>582</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>583</v>
+        <v>622</v>
       </c>
       <c r="Q5" s="7" t="s">
         <v>14</v>
@@ -4653,17 +4663,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0C00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -4970,17 +4980,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0D00-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0D00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5850,7 +5860,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7101,13 +7111,13 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="\\Resources\\hinh anh c6\\relay working animation.gif"/>
-    <hyperlink ref="B7" r:id="rId2" display="\\Resources\\hinh anh c6\\relay working animation.gif"/>
-    <hyperlink ref="B10" r:id="rId3" display="\\Resources\\mach c6.png"/>
-    <hyperlink ref="B11" r:id="rId4" display="\\Resources\\mach c6.png"/>
-    <hyperlink ref="B12" r:id="rId5" display="\\Resources\\mach c6.png"/>
-    <hyperlink ref="B8" r:id="rId6" display="\\Resources\\hinh anh c6\\relay working animation.gif"/>
-    <hyperlink ref="B9" r:id="rId7" display="\\Resources\\hinh anh c6\\relay working animation.gif"/>
+    <hyperlink ref="B6" r:id="rId1" display="\\Resources\\hinh anh c6\\relay working animation.gif" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId2" display="\\Resources\\hinh anh c6\\relay working animation.gif" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
+    <hyperlink ref="B10" r:id="rId3" display="\\Resources\\mach c6.png" xr:uid="{00000000-0004-0000-0F00-000002000000}"/>
+    <hyperlink ref="B11" r:id="rId4" display="\\Resources\\mach c6.png" xr:uid="{00000000-0004-0000-0F00-000003000000}"/>
+    <hyperlink ref="B12" r:id="rId5" display="\\Resources\\mach c6.png" xr:uid="{00000000-0004-0000-0F00-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="\\Resources\\hinh anh c6\\relay working animation.gif" xr:uid="{00000000-0004-0000-0F00-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="\\Resources\\hinh anh c6\\relay working animation.gif" xr:uid="{00000000-0004-0000-0F00-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -7115,7 +7125,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8253,30 +8263,30 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
-    <hyperlink ref="C7" r:id="rId4"/>
-    <hyperlink ref="C9" r:id="rId5"/>
-    <hyperlink ref="C10" r:id="rId6"/>
-    <hyperlink ref="C12" r:id="rId7"/>
-    <hyperlink ref="C11" r:id="rId8"/>
-    <hyperlink ref="C13" r:id="rId9"/>
-    <hyperlink ref="C14" r:id="rId10"/>
-    <hyperlink ref="C15" r:id="rId11"/>
-    <hyperlink ref="C16" r:id="rId12"/>
-    <hyperlink ref="C18" r:id="rId13"/>
-    <hyperlink ref="C19" r:id="rId14"/>
-    <hyperlink ref="C20" r:id="rId15"/>
-    <hyperlink ref="C21" r:id="rId16"/>
-    <hyperlink ref="C22" r:id="rId17"/>
-    <hyperlink ref="C24" r:id="rId18"/>
-    <hyperlink ref="C25" r:id="rId19" display="\\Resources\\Hinh anh cac chuong\\hinh anh c5\\short2ground.png"/>
-    <hyperlink ref="C30" r:id="rId20"/>
-    <hyperlink ref="C31" r:id="rId21"/>
-    <hyperlink ref="C32" r:id="rId22"/>
-    <hyperlink ref="C33" r:id="rId23"/>
-    <hyperlink ref="C2" r:id="rId24"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-1000-000001000000}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{00000000-0004-0000-1000-000002000000}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{00000000-0004-0000-1000-000003000000}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{00000000-0004-0000-1000-000004000000}"/>
+    <hyperlink ref="C10" r:id="rId6" xr:uid="{00000000-0004-0000-1000-000005000000}"/>
+    <hyperlink ref="C12" r:id="rId7" xr:uid="{00000000-0004-0000-1000-000006000000}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{00000000-0004-0000-1000-000007000000}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{00000000-0004-0000-1000-000008000000}"/>
+    <hyperlink ref="C14" r:id="rId10" xr:uid="{00000000-0004-0000-1000-000009000000}"/>
+    <hyperlink ref="C15" r:id="rId11" xr:uid="{00000000-0004-0000-1000-00000A000000}"/>
+    <hyperlink ref="C16" r:id="rId12" xr:uid="{00000000-0004-0000-1000-00000B000000}"/>
+    <hyperlink ref="C18" r:id="rId13" xr:uid="{00000000-0004-0000-1000-00000C000000}"/>
+    <hyperlink ref="C19" r:id="rId14" xr:uid="{00000000-0004-0000-1000-00000D000000}"/>
+    <hyperlink ref="C20" r:id="rId15" xr:uid="{00000000-0004-0000-1000-00000E000000}"/>
+    <hyperlink ref="C21" r:id="rId16" xr:uid="{00000000-0004-0000-1000-00000F000000}"/>
+    <hyperlink ref="C22" r:id="rId17" xr:uid="{00000000-0004-0000-1000-000010000000}"/>
+    <hyperlink ref="C24" r:id="rId18" xr:uid="{00000000-0004-0000-1000-000011000000}"/>
+    <hyperlink ref="C25" r:id="rId19" display="\\Resources\\Hinh anh cac chuong\\hinh anh c5\\short2ground.png" xr:uid="{00000000-0004-0000-1000-000012000000}"/>
+    <hyperlink ref="C30" r:id="rId20" xr:uid="{00000000-0004-0000-1000-000013000000}"/>
+    <hyperlink ref="C31" r:id="rId21" xr:uid="{00000000-0004-0000-1000-000014000000}"/>
+    <hyperlink ref="C32" r:id="rId22" xr:uid="{00000000-0004-0000-1000-000015000000}"/>
+    <hyperlink ref="C33" r:id="rId23" xr:uid="{00000000-0004-0000-1000-000016000000}"/>
+    <hyperlink ref="C2" r:id="rId24" xr:uid="{00000000-0004-0000-1000-000017000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId25"/>
@@ -8284,7 +8294,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8984,30 +8994,30 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8" display="\\Resources\Hinh anh cac chuong\hinh anh c6\wiring_final.png"/>
-    <hyperlink ref="B13" r:id="rId9" display="\\Resources\Hinh anh cac chuong\hinh anh c6\wiring_final.png"/>
-    <hyperlink ref="B14" r:id="rId10"/>
-    <hyperlink ref="B15" r:id="rId11"/>
-    <hyperlink ref="B16" r:id="rId12"/>
-    <hyperlink ref="B17" r:id="rId13"/>
-    <hyperlink ref="B18" r:id="rId14"/>
-    <hyperlink ref="B19" r:id="rId15"/>
-    <hyperlink ref="B20" r:id="rId16"/>
-    <hyperlink ref="B21" r:id="rId17"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-1100-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-1100-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-1100-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-1100-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-1100-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-1100-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" display="\\Resources\Hinh anh cac chuong\hinh anh c6\wiring_final.png" xr:uid="{00000000-0004-0000-1100-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" display="\\Resources\Hinh anh cac chuong\hinh anh c6\wiring_final.png" xr:uid="{00000000-0004-0000-1100-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{00000000-0004-0000-1100-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-1100-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{00000000-0004-0000-1100-00000B000000}"/>
+    <hyperlink ref="B17" r:id="rId13" xr:uid="{00000000-0004-0000-1100-00000C000000}"/>
+    <hyperlink ref="B18" r:id="rId14" xr:uid="{00000000-0004-0000-1100-00000D000000}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{00000000-0004-0000-1100-00000E000000}"/>
+    <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-1100-00000F000000}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{00000000-0004-0000-1100-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -9773,24 +9783,24 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG"/>
-    <hyperlink ref="B4" r:id="rId2" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG"/>
-    <hyperlink ref="B6" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="B13" r:id="rId9"/>
-    <hyperlink ref="B14" r:id="rId10"/>
-    <hyperlink ref="B15" r:id="rId11"/>
-    <hyperlink ref="B17" r:id="rId12"/>
-    <hyperlink ref="B18" r:id="rId13"/>
-    <hyperlink ref="B19" r:id="rId14"/>
-    <hyperlink ref="B20" r:id="rId15"/>
-    <hyperlink ref="B21" r:id="rId16"/>
-    <hyperlink ref="B22" r:id="rId17" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG"/>
-    <hyperlink ref="B23" r:id="rId18"/>
+    <hyperlink ref="B3" r:id="rId1" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-1200-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-1200-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-1200-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-1200-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-1200-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-1200-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-1200-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{00000000-0004-0000-1200-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-1200-00000A000000}"/>
+    <hyperlink ref="B17" r:id="rId12" xr:uid="{00000000-0004-0000-1200-00000B000000}"/>
+    <hyperlink ref="B18" r:id="rId13" xr:uid="{00000000-0004-0000-1200-00000C000000}"/>
+    <hyperlink ref="B19" r:id="rId14" xr:uid="{00000000-0004-0000-1200-00000D000000}"/>
+    <hyperlink ref="B20" r:id="rId15" xr:uid="{00000000-0004-0000-1200-00000E000000}"/>
+    <hyperlink ref="B21" r:id="rId16" xr:uid="{00000000-0004-0000-1200-00000F000000}"/>
+    <hyperlink ref="B22" r:id="rId17" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG" xr:uid="{00000000-0004-0000-1200-000010000000}"/>
+    <hyperlink ref="B23" r:id="rId18" xr:uid="{00000000-0004-0000-1200-000011000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -9798,7 +9808,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -10309,12 +10319,12 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\1.PNG"/>
-    <hyperlink ref="C3" r:id="rId2" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\2.PNG"/>
-    <hyperlink ref="C4" r:id="rId3" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\3.PNG"/>
-    <hyperlink ref="C5" r:id="rId4" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\2.PNG"/>
-    <hyperlink ref="C6" r:id="rId5" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\5.PNG"/>
-    <hyperlink ref="C7" r:id="rId6" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\5.PNG"/>
+    <hyperlink ref="C2" r:id="rId1" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\1.PNG" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\2.PNG" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\3.PNG" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\2.PNG" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\5.PNG" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" display="\\Resources1\\Hinh anh cac chuong\\hinh anh c2\\5.PNG" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -10322,7 +10332,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -10696,18 +10706,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
@@ -11027,17 +11037,17 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView topLeftCell="I1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
@@ -11448,11 +11458,11 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -11460,7 +11470,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -11711,16 +11721,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -12023,9 +12033,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -12033,7 +12043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -12518,10 +12528,10 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -12529,7 +12539,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -13113,11 +13123,11 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>